<commit_message>
Use averaging within a timestep when > 1 year. Restrict summary output log to only show total landscape values.
</commit_message>
<xml_diff>
--- a/trunk/tests/37 Good Species Variable Estimates_ All Species.xlsx
+++ b/trunk/tests/37 Good Species Variable Estimates_ All Species.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BRM\LANDIS_II\GitCode\Extension-Output-Bird-Habitat\trunk\tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="18195" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="11940" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -14,7 +19,10 @@
     <sheet name="Species &quot;Batch 1&quot;" sheetId="1" r:id="rId5"/>
     <sheet name="Species &quot;Batch 2&quot;" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'27 "New" Good Model Species'!$B$1:$H$103</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -295,7 +303,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,13 +322,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -332,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -369,6 +392,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,6 +422,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -426,7 +473,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -461,7 +508,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -672,7 +719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C6:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -737,11 +784,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
@@ -760,7 +816,7 @@
       <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="20" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="11" t="s">
@@ -784,7 +840,7 @@
       <c r="F2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="21">
         <v>0.70387900000000003</v>
       </c>
       <c r="H2" s="2"/>
@@ -806,7 +862,7 @@
       <c r="F3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="21">
         <v>-5.4579999999999997E-2</v>
       </c>
       <c r="H3" s="2"/>
@@ -828,13 +884,12 @@
       <c r="F4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="21">
         <v>-3.6158830000000002</v>
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>4</v>
       </c>
@@ -850,13 +905,11 @@
       <c r="F5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="21">
         <v>-5.9437600000000002</v>
       </c>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+    </row>
+    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>5</v>
       </c>
@@ -869,16 +922,14 @@
       <c r="E6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="21">
         <v>0.38047999999999998</v>
       </c>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+    </row>
+    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>6</v>
       </c>
@@ -891,16 +942,14 @@
       <c r="E7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="21">
         <v>0.30651</v>
       </c>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+    </row>
+    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>7</v>
       </c>
@@ -916,13 +965,11 @@
       <c r="F8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="21">
         <v>0.87151000000000001</v>
       </c>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+    </row>
+    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>8</v>
       </c>
@@ -938,13 +985,11 @@
       <c r="F9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="21">
         <v>-0.35783700000000002</v>
       </c>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>9</v>
       </c>
@@ -960,13 +1005,11 @@
       <c r="F10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="21">
         <v>1.5192000000000001E-2</v>
       </c>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+    </row>
+    <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>10</v>
       </c>
@@ -982,13 +1025,11 @@
       <c r="F11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="21">
         <v>-1.111356</v>
       </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+    </row>
+    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>11</v>
       </c>
@@ -1004,13 +1045,11 @@
       <c r="F12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="21">
         <v>-0.72642300000000004</v>
       </c>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+    </row>
+    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>12</v>
       </c>
@@ -1026,13 +1065,11 @@
       <c r="F13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="21">
         <v>0.56321299999999996</v>
       </c>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+    </row>
+    <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>13</v>
       </c>
@@ -1048,13 +1085,11 @@
       <c r="F14" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="21">
         <v>-8.5869999999999993E-6</v>
       </c>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+    </row>
+    <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>14</v>
       </c>
@@ -1070,13 +1105,11 @@
       <c r="F15" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="21">
         <v>-0.2419</v>
       </c>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+    </row>
+    <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>15</v>
       </c>
@@ -1089,16 +1122,14 @@
       <c r="E16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="21">
         <v>0.39419999999999999</v>
       </c>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+    </row>
+    <row r="17" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>16</v>
       </c>
@@ -1114,13 +1145,11 @@
       <c r="F17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="21">
         <v>0.18160000000000001</v>
       </c>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+    </row>
+    <row r="18" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>17</v>
       </c>
@@ -1136,13 +1165,11 @@
       <c r="F18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="21">
         <v>0.69410000000000005</v>
       </c>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+    </row>
+    <row r="19" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>18</v>
       </c>
@@ -1158,13 +1185,11 @@
       <c r="F19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="21">
         <v>-4.4560000000000004</v>
       </c>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+    </row>
+    <row r="20" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>19</v>
       </c>
@@ -1180,13 +1205,11 @@
       <c r="F20" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="21">
         <v>0.19861999999999999</v>
       </c>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+    </row>
+    <row r="21" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>20</v>
       </c>
@@ -1202,13 +1225,11 @@
       <c r="F21" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="21">
         <v>-2.3552499999999998</v>
       </c>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+    </row>
+    <row r="22" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>21</v>
       </c>
@@ -1224,13 +1245,11 @@
       <c r="F22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="21">
         <v>-2.698169</v>
       </c>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+    </row>
+    <row r="23" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>22</v>
       </c>
@@ -1246,13 +1265,11 @@
       <c r="F23" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="21">
         <v>-4.283E-2</v>
       </c>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+    </row>
+    <row r="24" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>23</v>
       </c>
@@ -1268,13 +1285,11 @@
       <c r="F24" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G24" s="21">
         <v>0.46950199999999997</v>
       </c>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
+    </row>
+    <row r="25" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <v>24</v>
       </c>
@@ -1290,13 +1305,11 @@
       <c r="F25" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G25" s="21">
         <v>-0.55102099999999998</v>
       </c>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
+    </row>
+    <row r="26" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>25</v>
       </c>
@@ -1312,13 +1325,11 @@
       <c r="F26" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G26" s="21">
         <v>0.350221</v>
       </c>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
+    </row>
+    <row r="27" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>26</v>
       </c>
@@ -1334,13 +1345,11 @@
       <c r="F27" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="21">
         <v>-2.3547820000000002</v>
       </c>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
+    </row>
+    <row r="28" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>27</v>
       </c>
@@ -1356,13 +1365,11 @@
       <c r="F28" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="21">
         <v>0.59566699999999995</v>
       </c>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
+    </row>
+    <row r="29" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
         <v>28</v>
       </c>
@@ -1378,13 +1385,11 @@
       <c r="F29" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="21">
         <v>-3.5979999999999998E-2</v>
       </c>
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
+    </row>
+    <row r="30" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
         <v>29</v>
       </c>
@@ -1400,13 +1405,11 @@
       <c r="F30" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="21">
         <v>1.9859000000000002E-2</v>
       </c>
-      <c r="H30" s="2"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
+    </row>
+    <row r="31" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2">
         <v>30</v>
       </c>
@@ -1422,13 +1425,11 @@
       <c r="F31" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="21">
         <v>-1.2662599999999999</v>
       </c>
-      <c r="H31" s="2"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
+    </row>
+    <row r="32" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
         <v>31</v>
       </c>
@@ -1444,13 +1445,11 @@
       <c r="F32" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G32" s="7">
+      <c r="G32" s="21">
         <v>-0.48283999999999999</v>
       </c>
-      <c r="H32" s="2"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
+    </row>
+    <row r="33" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
         <v>32</v>
       </c>
@@ -1466,13 +1465,11 @@
       <c r="F33" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G33" s="7">
+      <c r="G33" s="21">
         <v>-0.33201999999999998</v>
       </c>
-      <c r="H33" s="2"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
+    </row>
+    <row r="34" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="2">
         <v>33</v>
       </c>
@@ -1488,13 +1485,11 @@
       <c r="F34" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G34" s="7">
+      <c r="G34" s="21">
         <v>0.25635999999999998</v>
       </c>
-      <c r="H34" s="2"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
+    </row>
+    <row r="35" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
         <v>34</v>
       </c>
@@ -1510,13 +1505,11 @@
       <c r="F35" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="7">
+      <c r="G35" s="21">
         <v>-3.0927440000000002</v>
       </c>
-      <c r="H35" s="2"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
+    </row>
+    <row r="36" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <v>35</v>
       </c>
@@ -1532,13 +1525,11 @@
       <c r="F36" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G36" s="7">
+      <c r="G36" s="21">
         <v>-3.9919999999999997E-2</v>
       </c>
-      <c r="H36" s="2"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
+    </row>
+    <row r="37" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
         <v>36</v>
       </c>
@@ -1554,13 +1545,11 @@
       <c r="F37" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G37" s="7">
+      <c r="G37" s="21">
         <v>-1.2198910000000001</v>
       </c>
-      <c r="H37" s="2"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
+    </row>
+    <row r="38" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
         <v>37</v>
       </c>
@@ -1576,13 +1565,11 @@
       <c r="F38" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G38" s="8">
+      <c r="G38" s="21">
         <v>0.46211000000000002</v>
       </c>
-      <c r="H38" s="2"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
+    </row>
+    <row r="39" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
         <v>38</v>
       </c>
@@ -1598,13 +1585,11 @@
       <c r="F39" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G39" s="8">
+      <c r="G39" s="21">
         <v>-0.48953000000000002</v>
       </c>
-      <c r="H39" s="2"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
+    </row>
+    <row r="40" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="2">
         <v>39</v>
       </c>
@@ -1620,13 +1605,11 @@
       <c r="F40" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G40" s="8">
+      <c r="G40" s="21">
         <v>0.61531999999999998</v>
       </c>
-      <c r="H40" s="2"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
+    </row>
+    <row r="41" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
         <v>40</v>
       </c>
@@ -1642,13 +1625,11 @@
       <c r="F41" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G41" s="8">
+      <c r="G41" s="21">
         <v>-2.0067300000000001</v>
       </c>
-      <c r="H41" s="2"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
+    </row>
+    <row r="42" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
         <v>41</v>
       </c>
@@ -1664,13 +1645,11 @@
       <c r="F42" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G42" s="7">
+      <c r="G42" s="21">
         <v>1.19815</v>
       </c>
-      <c r="H42" s="2"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
+    </row>
+    <row r="43" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="2">
         <v>42</v>
       </c>
@@ -1686,13 +1665,11 @@
       <c r="F43" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G43" s="7">
+      <c r="G43" s="21">
         <v>-0.79901</v>
       </c>
-      <c r="H43" s="2"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
+    </row>
+    <row r="44" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="2">
         <v>43</v>
       </c>
@@ -1708,13 +1685,11 @@
       <c r="F44" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G44" s="7">
+      <c r="G44" s="21">
         <v>-0.48820000000000002</v>
       </c>
-      <c r="H44" s="2"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
+    </row>
+    <row r="45" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
         <v>44</v>
       </c>
@@ -1730,13 +1705,11 @@
       <c r="F45" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G45" s="7">
+      <c r="G45" s="21">
         <v>-3.27657</v>
       </c>
-      <c r="H45" s="2"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
+    </row>
+    <row r="46" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="2">
         <v>45</v>
       </c>
@@ -1752,13 +1725,11 @@
       <c r="F46" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G46" s="7">
+      <c r="G46" s="21">
         <v>0.48409999999999997</v>
       </c>
-      <c r="H46" s="2"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
+    </row>
+    <row r="47" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
         <v>46</v>
       </c>
@@ -1774,13 +1745,11 @@
       <c r="F47" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G47" s="7">
+      <c r="G47" s="21">
         <v>0.51992000000000005</v>
       </c>
-      <c r="H47" s="2"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
+    </row>
+    <row r="48" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="2">
         <v>47</v>
       </c>
@@ -1796,13 +1765,11 @@
       <c r="F48" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G48" s="7">
+      <c r="G48" s="21">
         <v>-0.36471999999999999</v>
       </c>
-      <c r="H48" s="2"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
+    </row>
+    <row r="49" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2">
         <v>48</v>
       </c>
@@ -1818,13 +1785,11 @@
       <c r="F49" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G49" s="7">
+      <c r="G49" s="21">
         <v>0.38294</v>
       </c>
-      <c r="H49" s="2"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="2"/>
+    </row>
+    <row r="50" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2">
         <v>49</v>
       </c>
@@ -1840,13 +1805,11 @@
       <c r="F50" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G50" s="7">
+      <c r="G50" s="21">
         <v>-3.0533100000000002</v>
       </c>
-      <c r="H50" s="2"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
+    </row>
+    <row r="51" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="2">
         <v>50</v>
       </c>
@@ -1862,13 +1825,11 @@
       <c r="F51" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G51" s="7">
+      <c r="G51" s="21">
         <v>1.6959999999999999E-2</v>
       </c>
-      <c r="H51" s="2"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
+    </row>
+    <row r="52" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="2">
         <v>51</v>
       </c>
@@ -1884,13 +1845,11 @@
       <c r="F52" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G52" s="7">
+      <c r="G52" s="21">
         <v>0.53241899999999998</v>
       </c>
-      <c r="H52" s="2"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
+    </row>
+    <row r="53" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="2">
         <v>52</v>
       </c>
@@ -1906,13 +1865,11 @@
       <c r="F53" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G53" s="7">
+      <c r="G53" s="21">
         <v>0.16839999999999999</v>
       </c>
-      <c r="H53" s="2"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="2"/>
+    </row>
+    <row r="54" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="2">
         <v>53</v>
       </c>
@@ -1928,13 +1885,11 @@
       <c r="F54" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G54" s="7">
+      <c r="G54" s="21">
         <v>0.41628599999999999</v>
       </c>
-      <c r="H54" s="2"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="2"/>
+    </row>
+    <row r="55" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="2">
         <v>54</v>
       </c>
@@ -1950,13 +1905,11 @@
       <c r="F55" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G55" s="7">
+      <c r="G55" s="21">
         <v>-3.7314430000000001</v>
       </c>
-      <c r="H55" s="2"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
+    </row>
+    <row r="56" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="2">
         <v>55</v>
       </c>
@@ -1972,13 +1925,11 @@
       <c r="F56" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G56" s="7">
+      <c r="G56" s="21">
         <v>-4.1319600000000003</v>
       </c>
-      <c r="H56" s="2"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="2"/>
+    </row>
+    <row r="57" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="2">
         <v>56</v>
       </c>
@@ -1994,13 +1945,11 @@
       <c r="F57" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G57" s="7">
+      <c r="G57" s="21">
         <v>0.25557999999999997</v>
       </c>
-      <c r="H57" s="2"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="2"/>
+    </row>
+    <row r="58" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="2">
         <v>57</v>
       </c>
@@ -2016,13 +1965,11 @@
       <c r="F58" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G58" s="7">
+      <c r="G58" s="21">
         <v>0.32541999999999999</v>
       </c>
-      <c r="H58" s="2"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="2"/>
+    </row>
+    <row r="59" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="2">
         <v>58</v>
       </c>
@@ -2038,13 +1985,11 @@
       <c r="F59" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G59" s="7">
+      <c r="G59" s="21">
         <v>1.2423</v>
       </c>
-      <c r="H59" s="2"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="2"/>
+    </row>
+    <row r="60" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="2">
         <v>59</v>
       </c>
@@ -2060,13 +2005,11 @@
       <c r="F60" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G60" s="7">
+      <c r="G60" s="21">
         <v>0.90980000000000005</v>
       </c>
-      <c r="H60" s="2"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="2"/>
+    </row>
+    <row r="61" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="2">
         <v>60</v>
       </c>
@@ -2082,12 +2025,11 @@
       <c r="F61" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G61" s="1">
+      <c r="G61" s="22">
         <v>-7.4283000000000001</v>
       </c>
-      <c r="H61" s="2"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2">
         <v>61</v>
       </c>
@@ -2103,14 +2045,14 @@
       <c r="F62" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G62" s="13">
+      <c r="G62" s="22">
         <v>-1.379E-5</v>
       </c>
       <c r="H62" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2">
         <v>62</v>
       </c>
@@ -2123,14 +2065,14 @@
       <c r="E63" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F63" s="4" t="s">
+      <c r="F63" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="G63" s="13">
+      <c r="G63" s="22">
         <v>-0.2455</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="2">
         <v>63</v>
       </c>
@@ -2146,11 +2088,11 @@
       <c r="F64" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G64" s="13">
+      <c r="G64" s="22">
         <v>0.24809999999999999</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="2">
         <v>64</v>
       </c>
@@ -2166,11 +2108,11 @@
       <c r="F65" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="G65" s="13">
+      <c r="G65" s="22">
         <v>0.31430000000000002</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="2">
         <v>65</v>
       </c>
@@ -2186,11 +2128,11 @@
       <c r="F66" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G66" s="13">
+      <c r="G66" s="22">
         <v>-2.048</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="2">
         <v>66</v>
       </c>
@@ -2203,14 +2145,14 @@
       <c r="E67" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F67" s="4" t="s">
+      <c r="F67" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="G67" s="14">
+      <c r="G67" s="22">
         <v>-0.97316000000000003</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="2">
         <v>67</v>
       </c>
@@ -2223,14 +2165,14 @@
       <c r="E68" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F68" s="4" t="s">
+      <c r="F68" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="G68" s="14">
+      <c r="G68" s="22">
         <v>0.81118999999999997</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="2">
         <v>68</v>
       </c>
@@ -2246,11 +2188,11 @@
       <c r="F69" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G69" s="14">
+      <c r="G69" s="22">
         <v>-4.4650000000000002E-2</v>
       </c>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="2">
         <v>69</v>
       </c>
@@ -2266,11 +2208,11 @@
       <c r="F70" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G70" s="14">
+      <c r="G70" s="22">
         <v>1.19624</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="2">
         <v>70</v>
       </c>
@@ -2286,14 +2228,14 @@
       <c r="F71" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G71" s="15">
+      <c r="G71" s="23">
         <v>-5.85534</v>
       </c>
       <c r="H71" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="2">
         <v>71</v>
       </c>
@@ -2309,14 +2251,14 @@
       <c r="F72" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G72" s="2">
+      <c r="G72" s="23">
         <v>-5.4039999999999998E-2</v>
       </c>
       <c r="H72" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="2">
         <v>72</v>
       </c>
@@ -2332,14 +2274,14 @@
       <c r="F73" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G73" s="2">
+      <c r="G73" s="23">
         <v>0.89742</v>
       </c>
       <c r="H73" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="2">
         <v>73</v>
       </c>
@@ -2355,14 +2297,14 @@
       <c r="F74" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G74" s="14">
+      <c r="G74" s="22">
         <v>-3.8224939999999998</v>
       </c>
       <c r="H74" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="2">
         <v>74</v>
       </c>
@@ -2378,14 +2320,14 @@
       <c r="F75" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G75" s="14">
+      <c r="G75" s="22">
         <v>-4.6851999999999998E-2</v>
       </c>
       <c r="H75" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="2">
         <v>75</v>
       </c>
@@ -2401,14 +2343,14 @@
       <c r="F76" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G76" s="14">
+      <c r="G76" s="22">
         <v>0.65975499999999998</v>
       </c>
       <c r="H76" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="2">
         <v>76</v>
       </c>
@@ -2424,11 +2366,11 @@
       <c r="F77" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G77" s="13">
+      <c r="G77" s="22">
         <v>0.18944</v>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="2">
         <v>77</v>
       </c>
@@ -2444,11 +2386,11 @@
       <c r="F78" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G78" s="13">
+      <c r="G78" s="22">
         <v>-0.42060999999999998</v>
       </c>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="2">
         <v>78</v>
       </c>
@@ -2464,11 +2406,11 @@
       <c r="F79" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G79" s="13">
+      <c r="G79" s="22">
         <v>-0.46578999999999998</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="2">
         <v>79</v>
       </c>
@@ -2484,103 +2426,103 @@
       <c r="F80" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G80" s="13">
+      <c r="G80" s="22">
         <v>7.5560000000000002E-2</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B81" s="2">
+    <row r="81" spans="2:8" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="28">
         <v>80</v>
       </c>
-      <c r="C81" s="4" t="s">
+      <c r="C81" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="D81" s="4">
-        <v>200</v>
-      </c>
-      <c r="E81" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F81" s="4" t="s">
+      <c r="D81" s="29">
+        <v>200</v>
+      </c>
+      <c r="E81" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F81" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="G81" s="14">
+      <c r="G81" s="30">
         <v>0.19563</v>
       </c>
-      <c r="H81" s="4" t="s">
+      <c r="H81" s="29" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B82" s="2">
+    <row r="82" spans="2:8" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="28">
         <v>81</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="C82" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="D82" s="4">
+      <c r="D82" s="29">
         <v>500</v>
       </c>
-      <c r="E82" s="4" t="s">
+      <c r="E82" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F82" s="4" t="s">
+      <c r="F82" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="G82" s="14">
+      <c r="G82" s="30">
         <v>0.64654999999999996</v>
       </c>
-      <c r="H82" s="4" t="s">
+      <c r="H82" s="29" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="2">
+    <row r="83" spans="2:8" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="28">
         <v>82</v>
       </c>
-      <c r="C83" s="4" t="s">
+      <c r="C83" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="D83" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F83" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G83" s="14">
+      <c r="D83" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F83" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G83" s="30">
         <v>-3.8907699999999998</v>
       </c>
-      <c r="H83" s="4" t="s">
+      <c r="H83" s="29" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B84" s="2">
+    <row r="84" spans="2:8" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="28">
         <v>83</v>
       </c>
-      <c r="C84" s="4" t="s">
+      <c r="C84" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="D84" s="4">
+      <c r="D84" s="29">
         <v>100</v>
       </c>
-      <c r="E84" s="4" t="s">
+      <c r="E84" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="F84" s="4" t="s">
+      <c r="F84" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="G84" s="14">
+      <c r="G84" s="30">
         <v>-9.7441999999999997E-3</v>
       </c>
-      <c r="H84" s="4" t="s">
+      <c r="H84" s="29" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B85" s="2">
         <v>84</v>
       </c>
@@ -2596,14 +2538,14 @@
       <c r="F85" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G85" s="14">
+      <c r="G85" s="22">
         <v>1.1560824000000001</v>
       </c>
       <c r="H85" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B86" s="2">
         <v>85</v>
       </c>
@@ -2619,14 +2561,14 @@
       <c r="F86" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G86" s="14">
+      <c r="G86" s="22">
         <v>-6.3263296000000002</v>
       </c>
       <c r="H86" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B87" s="2">
         <v>86</v>
       </c>
@@ -2642,11 +2584,11 @@
       <c r="F87" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G87" s="14">
+      <c r="G87" s="22">
         <v>-1.4378999999999999E-2</v>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B88" s="2">
         <v>87</v>
       </c>
@@ -2662,11 +2604,11 @@
       <c r="F88" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G88" s="14">
+      <c r="G88" s="22">
         <v>0.28651700000000002</v>
       </c>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B89" s="2">
         <v>88</v>
       </c>
@@ -2682,11 +2624,11 @@
       <c r="F89" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G89" s="14">
+      <c r="G89" s="22">
         <v>0.24704100000000001</v>
       </c>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B90" s="2">
         <v>89</v>
       </c>
@@ -2702,11 +2644,11 @@
       <c r="F90" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G90" s="14">
+      <c r="G90" s="22">
         <v>0.88197300000000001</v>
       </c>
     </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B91" s="2">
         <v>90</v>
       </c>
@@ -2722,11 +2664,11 @@
       <c r="F91" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G91" s="14">
+      <c r="G91" s="22">
         <v>-4.2427929999999998</v>
       </c>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B92" s="2">
         <v>91</v>
       </c>
@@ -2742,11 +2684,11 @@
       <c r="F92" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G92" s="4">
+      <c r="G92" s="24">
         <v>-1.4863700000000001E-2</v>
       </c>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B93" s="2">
         <v>92</v>
       </c>
@@ -2762,11 +2704,11 @@
       <c r="F93" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G93" s="4">
+      <c r="G93" s="24">
         <v>0.4530769</v>
       </c>
     </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B94" s="2">
         <v>93</v>
       </c>
@@ -2782,11 +2724,11 @@
       <c r="F94" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G94" s="4">
+      <c r="G94" s="24">
         <v>-0.10464329999999999</v>
       </c>
     </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B95" s="2">
         <v>94</v>
       </c>
@@ -2802,11 +2744,11 @@
       <c r="F95" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G95" s="4">
+      <c r="G95" s="24">
         <v>-2.8251509000000001</v>
       </c>
     </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B96" s="2">
         <v>95</v>
       </c>
@@ -2822,11 +2764,11 @@
       <c r="F96" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G96" s="13">
+      <c r="G96" s="22">
         <v>-3.0831499999999998</v>
       </c>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B97" s="2">
         <v>96</v>
       </c>
@@ -2842,11 +2784,11 @@
       <c r="F97" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G97" s="13">
+      <c r="G97" s="22">
         <v>1.57921</v>
       </c>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B98" s="2">
         <v>97</v>
       </c>
@@ -2862,11 +2804,11 @@
       <c r="F98" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G98" s="13">
+      <c r="G98" s="22">
         <v>-0.16552</v>
       </c>
     </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B99" s="2">
         <v>98</v>
       </c>
@@ -2882,11 +2824,11 @@
       <c r="F99" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G99" s="13">
+      <c r="G99" s="22">
         <v>-1.4353199999999999</v>
       </c>
     </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B100" s="2">
         <v>99</v>
       </c>
@@ -2902,11 +2844,11 @@
       <c r="F100" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G100" s="13">
+      <c r="G100" s="22">
         <v>3.261E-2</v>
       </c>
     </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B101" s="2">
         <v>100</v>
       </c>
@@ -2922,14 +2864,14 @@
       <c r="F101" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G101" s="13">
+      <c r="G101" s="22">
         <v>-8.25</v>
       </c>
       <c r="H101" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B102" s="2">
         <v>101</v>
       </c>
@@ -2945,14 +2887,14 @@
       <c r="F102" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G102" s="13">
+      <c r="G102" s="22">
         <v>1.9219999999999999</v>
       </c>
       <c r="H102" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B103" s="2">
         <v>102</v>
       </c>
@@ -2968,7 +2910,7 @@
       <c r="F103" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G103" s="13">
+      <c r="G103" s="22">
         <v>-1.47E-3</v>
       </c>
       <c r="H103" s="4" t="s">
@@ -2977,6 +2919,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>